<commit_message>
feat: Add 'Report Problem' test suite, page object, and data, along with updates to calculation files.
</commit_message>
<xml_diff>
--- a/test-contract-data/BRPUTBW81519.xlsx
+++ b/test-contract-data/BRPUTBW81519.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -620,10 +620,10 @@
         <v>81.35</v>
       </c>
       <c r="K4">
-        <v>1382.9499999999998</v>
+        <v>1482.95</v>
       </c>
       <c r="L4">
-        <v>1148.02</v>
+        <v>1248.02</v>
       </c>
       <c r="M4" t="str">
         <v>-</v>
@@ -697,165 +697,9 @@
         <v>$84.35  05/21/2024  	  First Recurring Payment     	  Paid  Visa 1111</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>After First Recurring</v>
-      </c>
-      <c r="B10" t="str">
-        <v>BRPUTBW81519</v>
-      </c>
-      <c r="C10" t="str">
-        <v>-</v>
-      </c>
-      <c r="D10" t="str">
-        <v>-</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>16.99</v>
-      </c>
-      <c r="G10" t="str">
-        <v>-</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>66.66666666666667</v>
-      </c>
-      <c r="J10">
-        <v>81.35</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>14.68</v>
-      </c>
-      <c r="M10" t="str">
-        <v>-</v>
-      </c>
-      <c r="N10">
-        <v>18</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="str">
-        <v>-</v>
-      </c>
-      <c r="R10" t="str">
-        <v>-</v>
-      </c>
-      <c r="S10">
-        <v>345.556873465787</v>
-      </c>
-      <c r="T10" t="str">
-        <v>-</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Transaction History</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Amount</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Description</v>
-      </c>
-      <c r="D13" t="str">
-        <v>Full Text</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>05/21/2024</v>
-      </c>
-      <c r="B14">
-        <v>123.35</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Denefits Fee + Upfront Payment Paid Visa 1111</v>
-      </c>
-      <c r="D14" t="str">
-        <v>$123.35  05/21/2024  	  Denefits Fee + Upfront Payment     	  Paid  Visa 1111</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>05/21/2024</v>
-      </c>
-      <c r="B15">
-        <v>84.35</v>
-      </c>
-      <c r="C15" t="str">
-        <v>First Recurring Payment Paid Visa 1111</v>
-      </c>
-      <c r="D15" t="str">
-        <v>$84.35  05/21/2024  	  First Recurring Payment     	  Paid  Visa 1111</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Transaction History</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Amount</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Description</v>
-      </c>
-      <c r="D18" t="str">
-        <v>Full Text</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>05/21/2024</v>
-      </c>
-      <c r="B19">
-        <v>123.35</v>
-      </c>
-      <c r="C19" t="str">
-        <v>Denefits Fee + Upfront Payment Paid Visa 1111</v>
-      </c>
-      <c r="D19" t="str">
-        <v>$123.35  05/21/2024  	  Denefits Fee + Upfront Payment     	  Paid  Visa 1111</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>05/21/2024</v>
-      </c>
-      <c r="B20">
-        <v>84.35</v>
-      </c>
-      <c r="C20" t="str">
-        <v>First Recurring Payment Paid Visa 1111</v>
-      </c>
-      <c r="D20" t="str">
-        <v>$84.35  05/21/2024  	  First Recurring Payment     	  Paid  Visa 1111</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add Profile page object and test suite, update test utilities, and clean up old Allure test results.
</commit_message>
<xml_diff>
--- a/test-contract-data/BRPUTBW81519.xlsx
+++ b/test-contract-data/BRPUTBW81519.xlsx
@@ -611,7 +611,7 @@
         <v>-</v>
       </c>
       <c r="H4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>66.66666666666667</v>
@@ -623,7 +623,7 @@
         <v>1482.95</v>
       </c>
       <c r="L4">
-        <v>1248.02</v>
+        <v>1262.7</v>
       </c>
       <c r="M4" t="str">
         <v>-</v>

</xml_diff>